<commit_message>
Worked on models and subject service
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sashi\Desktop\Development\LearningSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA543CF-A9D3-4C77-8BE4-BA071B50DF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F024B55A-ABB5-4B2A-ADA4-5294E97FF8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Basic database setup</t>
   </si>
@@ -37,6 +37,39 @@
   </si>
   <si>
     <t>Go through migrations in Laravel again</t>
+  </si>
+  <si>
+    <t>Complete basic migration setup</t>
+  </si>
+  <si>
+    <t>Adjust career model file with pk and relationships</t>
+  </si>
+  <si>
+    <t>Create career service</t>
+  </si>
+  <si>
+    <t>Add in dummy methods for reading careers, creating careers and editing careers</t>
+  </si>
+  <si>
+    <t>Add logic for creating a career</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Add logic for reading careers</t>
+  </si>
+  <si>
+    <t>Create a user service</t>
+  </si>
+  <si>
+    <t>Add methods shells for basic crud operations</t>
+  </si>
+  <si>
+    <t>Add create method logic</t>
   </si>
 </sst>
 </file>
@@ -52,12 +85,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,18 +412,93 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>